<commit_message>
adding tags - more checks needed
</commit_message>
<xml_diff>
--- a/Realms_Config.xlsx
+++ b/Realms_Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul\Documents\staas-provisioning-fusion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDA429B-589D-408E-8525-B49CD3943B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539BA59E-EF4E-4C2B-A6E4-A4F1BF6DCDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="45315" windowHeight="23911" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,7 +385,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>